<commit_message>
latest push on UnitID fixed
</commit_message>
<xml_diff>
--- a/data/DestinationTables.xlsx
+++ b/data/DestinationTables.xlsx
@@ -11187,7 +11187,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
@@ -11222,7 +11222,7 @@
         </is>
       </c>
     </row>
-    <row r="2" hidden="1" ht="14.25" customHeight="1">
+    <row r="2" ht="14.25" customHeight="1">
       <c r="A2" s="15" t="n">
         <v>1</v>
       </c>
@@ -11260,7 +11260,7 @@
       <c r="Y2" s="5" t="n"/>
       <c r="Z2" s="5" t="n"/>
     </row>
-    <row r="3" hidden="1" ht="14.25" customHeight="1">
+    <row r="3" ht="14.25" customHeight="1">
       <c r="A3" s="15" t="n">
         <v>2</v>
       </c>
@@ -11336,7 +11336,7 @@
       <c r="Y4" s="3" t="n"/>
       <c r="Z4" s="3" t="n"/>
     </row>
-    <row r="5" hidden="1" ht="14.25" customHeight="1">
+    <row r="5" ht="14.25" customHeight="1">
       <c r="A5" s="15" t="n">
         <v>4</v>
       </c>
@@ -11374,7 +11374,7 @@
       <c r="Y5" s="5" t="n"/>
       <c r="Z5" s="5" t="n"/>
     </row>
-    <row r="6" hidden="1" ht="14.25" customHeight="1">
+    <row r="6" ht="14.25" customHeight="1">
       <c r="A6" s="15" t="n">
         <v>5</v>
       </c>
@@ -11412,7 +11412,7 @@
       <c r="Y6" s="5" t="n"/>
       <c r="Z6" s="5" t="n"/>
     </row>
-    <row r="7" hidden="1" ht="14.25" customHeight="1">
+    <row r="7" ht="14.25" customHeight="1">
       <c r="A7" s="15" t="n">
         <v>6</v>
       </c>
@@ -11450,7 +11450,7 @@
       <c r="Y7" s="5" t="n"/>
       <c r="Z7" s="5" t="n"/>
     </row>
-    <row r="8" hidden="1" ht="14.25" customHeight="1">
+    <row r="8" ht="14.25" customHeight="1">
       <c r="A8" s="16" t="n">
         <v>7</v>
       </c>
@@ -11488,7 +11488,7 @@
       <c r="Y8" s="3" t="n"/>
       <c r="Z8" s="3" t="n"/>
     </row>
-    <row r="9" hidden="1" ht="14.25" customHeight="1">
+    <row r="9" ht="14.25" customHeight="1">
       <c r="A9" s="15" t="n">
         <v>8</v>
       </c>
@@ -11526,7 +11526,7 @@
       <c r="Y9" s="5" t="n"/>
       <c r="Z9" s="5" t="n"/>
     </row>
-    <row r="10" hidden="1" ht="14.25" customHeight="1">
+    <row r="10" ht="14.25" customHeight="1">
       <c r="A10" s="15" t="n">
         <v>9</v>
       </c>
@@ -11564,7 +11564,7 @@
       <c r="Y10" s="5" t="n"/>
       <c r="Z10" s="5" t="n"/>
     </row>
-    <row r="11" hidden="1" ht="14.25" customHeight="1">
+    <row r="11" ht="14.25" customHeight="1">
       <c r="A11" s="15" t="n">
         <v>10</v>
       </c>
@@ -11602,7 +11602,7 @@
       <c r="Y11" s="5" t="n"/>
       <c r="Z11" s="5" t="n"/>
     </row>
-    <row r="12" hidden="1" ht="14.25" customHeight="1">
+    <row r="12" ht="14.25" customHeight="1">
       <c r="A12" s="16" t="n">
         <v>11</v>
       </c>
@@ -12709,16 +12709,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:C15">
-    <filterColumn colId="1" hiddenButton="0" showButton="1">
-      <filters>
-        <filter val="cubic meters"/>
-        <filter val="euros"/>
-        <filter val="kWh"/>
-        <filter val="us dollars"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C15"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>